<commit_message>
raccolti dati ampiezza distanza
</commit_message>
<xml_diff>
--- a/20240509micoonde/dati_microonde.xlsx
+++ b/20240509micoonde/dati_microonde.xlsx
@@ -3,17 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="malus" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ampiezza angolo" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ampiezza distanza" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Emettitore</t>
   </si>
@@ -52,29 +54,96 @@
   </si>
   <si>
     <t>x30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">teta (deg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V (Volt) NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sigmaV NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90 (piede)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56 (pancia)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ricevitore MIN (piede) (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vmin (Volt)</t>
+  </si>
+  <si>
+    <t>sigmaVmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ricevitore MAX (piede) (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vmax (Volt)</t>
+  </si>
+  <si>
+    <t>sigmaVmax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emettitore (piede) (cm)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.000000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor theme="9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,17 +155,38 @@
       <diagonal style="none"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="2" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="164" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf fontId="2" fillId="4" borderId="0" numFmtId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
+    <cellStyle name="Accent6" xfId="3" builtinId="49"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -880,4 +970,704 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="13.00390625"/>
+    <col customWidth="1" min="3" max="3" width="12.8515625"/>
+    <col customWidth="1" min="4" max="4" width="14.28125"/>
+    <col customWidth="1" min="5" max="5" width="15.8515625"/>
+    <col customWidth="1" min="6" max="6" width="11.8515625"/>
+    <col customWidth="1" min="7" max="7" width="19.7109375"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6">
+        <v>3.5499999999999998</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="D2" s="7">
+        <v>4.6200000000000001</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>10</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2.7000000000000002</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="D3" s="7">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1.1799999999999999</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.85999999999999999</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.20000000000000001</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.31</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.059999999999999998</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.0050000000000000001</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.050000000000000003</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>-10</v>
+      </c>
+      <c r="B8" s="6">
+        <v>3.0499999999999998</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.029999999999999999</v>
+      </c>
+      <c r="D8" s="7">
+        <v>3.6899999999999999</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>-20</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1.6799999999999999</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1.8899999999999999</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>-30</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>-40</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.29999999999999999</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.19</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>-50</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.11</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.029999999999999999</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="24.00390625"/>
+    <col customWidth="1" min="4" max="4" width="30.8515625"/>
+    <col customWidth="1" min="5" max="6" width="11.7109375"/>
+    <col customWidth="1" min="7" max="7" width="17.28125"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1"/>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="10">
+        <v>54</v>
+      </c>
+      <c r="B2" s="7">
+        <v>3.3399999999999999</v>
+      </c>
+      <c r="C2" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="D2" s="11">
+        <v>53.299999999999997</v>
+      </c>
+      <c r="E2" s="12">
+        <v>3.5299999999999998</v>
+      </c>
+      <c r="F2" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="10">
+        <v>52.600000000000001</v>
+      </c>
+      <c r="B3" s="7">
+        <v>3.27</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="D3" s="11">
+        <v>51.899999999999999</v>
+      </c>
+      <c r="E3" s="12">
+        <v>3.3799999999999999</v>
+      </c>
+      <c r="F3" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="G3" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="10">
+        <v>51.200000000000003</v>
+      </c>
+      <c r="B4" s="7">
+        <v>3.2000000000000002</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="D4" s="11">
+        <v>50.5</v>
+      </c>
+      <c r="E4" s="12">
+        <v>3.2799999999999998</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="G4" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="10">
+        <v>49.799999999999997</v>
+      </c>
+      <c r="B5" s="7">
+        <v>3.1299999999999999</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="D5" s="11">
+        <v>49.100000000000001</v>
+      </c>
+      <c r="E5" s="12">
+        <v>3.2000000000000002</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="G5" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="10">
+        <v>48.399999999999999</v>
+      </c>
+      <c r="B6" s="7">
+        <v>3.0499999999999998</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="10">
+        <v>47.700000000000003</v>
+      </c>
+      <c r="E6" s="7">
+        <v>3.1000000000000001</v>
+      </c>
+      <c r="F6" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="G6" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="10">
+        <v>47</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2.9399999999999999</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="D7" s="10">
+        <v>46.299999999999997</v>
+      </c>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="G7" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="10">
+        <v>45.600000000000001</v>
+      </c>
+      <c r="B8" s="7">
+        <v>2.8500000000000001</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="D8" s="10">
+        <v>45</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1.9199999999999999</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G8" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="10">
+        <v>44.200000000000003</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2.7400000000000002</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="D9" s="10">
+        <v>43.5</v>
+      </c>
+      <c r="E9" s="7">
+        <v>2.8199999999999998</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G9" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="13">
+        <v>46.799999999999997</v>
+      </c>
+      <c r="B10" s="14">
+        <v>4.1299999999999999</v>
+      </c>
+      <c r="C10" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="D10" s="10">
+        <v>47.5</v>
+      </c>
+      <c r="E10" s="7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="13">
+        <v>45.399999999999999</v>
+      </c>
+      <c r="B11" s="14">
+        <v>4.0300000000000002</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="D11" s="10">
+        <v>46.100000000000001</v>
+      </c>
+      <c r="E11" s="7">
+        <v>4.6799999999999997</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="13">
+        <v>44</v>
+      </c>
+      <c r="B12" s="14">
+        <v>3.96</v>
+      </c>
+      <c r="C12" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="D12" s="10">
+        <v>44.600000000000001</v>
+      </c>
+      <c r="E12" s="7">
+        <v>4.54</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="G12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="13">
+        <v>42.5</v>
+      </c>
+      <c r="B13" s="14">
+        <v>3.8100000000000001</v>
+      </c>
+      <c r="C13" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="D13" s="10">
+        <v>43.299999999999997</v>
+      </c>
+      <c r="E13" s="7">
+        <v>4.3799999999999999</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="13">
+        <v>41</v>
+      </c>
+      <c r="B14" s="14">
+        <v>3.7599999999999998</v>
+      </c>
+      <c r="C14" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="D14" s="10">
+        <v>41.899999999999999</v>
+      </c>
+      <c r="E14" s="7">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="G14">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="13">
+        <v>39.600000000000001</v>
+      </c>
+      <c r="B15" s="14">
+        <v>3.6800000000000002</v>
+      </c>
+      <c r="C15" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="D15" s="10">
+        <v>40.399999999999999</v>
+      </c>
+      <c r="E15" s="7">
+        <v>4.25</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="13">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="B16" s="14">
+        <v>3.5499999999999998</v>
+      </c>
+      <c r="C16" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="D16" s="10">
+        <v>38.899999999999999</v>
+      </c>
+      <c r="E16" s="7">
+        <v>4.04</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="13">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="B17" s="14">
+        <v>3.4700000000000002</v>
+      </c>
+      <c r="C17" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="D17" s="10">
+        <v>37.5</v>
+      </c>
+      <c r="E17" s="7">
+        <v>3.8500000000000001</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G17">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="13">
+        <v>35.399999999999999</v>
+      </c>
+      <c r="B18" s="14">
+        <v>3.3900000000000001</v>
+      </c>
+      <c r="C18" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="D18" s="10">
+        <v>36</v>
+      </c>
+      <c r="E18" s="7">
+        <v>3.7000000000000002</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G18">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="D19" s="10">
+        <v>34.600000000000001</v>
+      </c>
+      <c r="E19" s="7">
+        <v>3.6200000000000001</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="G19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25"/>
+    <row r="21" ht="14.25"/>
+    <row r="22" ht="14.25"/>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ampiezza riprendiamo i dati perchè la dipendenza non è 1/r
</commit_message>
<xml_diff>
--- a/20240509micoonde/dati_microonde.xlsx
+++ b/20240509micoonde/dati_microonde.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Emettitore</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t xml:space="preserve">Emettitore (piede) (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX (cm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vmax (volt)</t>
+  </si>
+  <si>
+    <t>80cm</t>
   </si>
 </sst>
 </file>
@@ -100,7 +109,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -119,8 +128,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.000000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +160,12 @@
         <bgColor theme="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -155,26 +176,25 @@
       <diagonal style="none"/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="2" fillId="4" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
+    <xf fontId="3" fillId="5" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="164" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf fontId="2" fillId="4" borderId="0" numFmtId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf fontId="3" fillId="5" borderId="0" numFmtId="0" xfId="4" applyFont="1" applyFill="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="165" xfId="0" applyNumberFormat="1">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -182,11 +202,12 @@
       <protection hidden="0" locked="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Accent6" xfId="3" builtinId="49"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -979,7 +1000,7 @@
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="13.00390625"/>
     <col customWidth="1" min="3" max="3" width="12.8515625"/>
@@ -999,10 +1020,10 @@
       <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -1016,13 +1037,13 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>3.5499999999999998</v>
       </c>
       <c r="C2" s="4">
         <v>0.01</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>4.6200000000000001</v>
       </c>
       <c r="E2" s="3">
@@ -1039,13 +1060,13 @@
       <c r="A3">
         <v>10</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>2.7000000000000002</v>
       </c>
       <c r="C3" s="4">
         <v>0.01</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>4.1900000000000004</v>
       </c>
       <c r="E3" s="3">
@@ -1056,13 +1077,13 @@
       <c r="A4">
         <v>20</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>1.1799999999999999</v>
       </c>
       <c r="C4" s="4">
         <v>0.01</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>2.2599999999999998</v>
       </c>
       <c r="E4" s="3">
@@ -1073,13 +1094,13 @@
       <c r="A5">
         <v>30</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0.56000000000000005</v>
       </c>
       <c r="C5" s="4">
         <v>0.01</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>0.85999999999999999</v>
       </c>
       <c r="E5" s="3">
@@ -1090,13 +1111,13 @@
       <c r="A6">
         <v>40</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>0.20000000000000001</v>
       </c>
       <c r="C6" s="4">
         <v>0.01</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="6">
         <v>0.31</v>
       </c>
       <c r="E6" s="3">
@@ -1107,13 +1128,13 @@
       <c r="A7">
         <v>50</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>0.059999999999999998</v>
       </c>
       <c r="C7" s="4">
         <v>0.0050000000000000001</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>0.050000000000000003</v>
       </c>
       <c r="E7" s="3">
@@ -1124,13 +1145,13 @@
       <c r="A8">
         <v>-10</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>3.0499999999999998</v>
       </c>
       <c r="C8" s="4">
         <v>0.029999999999999999</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>3.6899999999999999</v>
       </c>
       <c r="E8" s="3">
@@ -1141,13 +1162,13 @@
       <c r="A9">
         <v>-20</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>1.6799999999999999</v>
       </c>
       <c r="C9" s="4">
         <v>0.02</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>1.8899999999999999</v>
       </c>
       <c r="E9" s="3">
@@ -1158,13 +1179,13 @@
       <c r="A10">
         <v>-30</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>0.75</v>
       </c>
       <c r="C10" s="4">
         <v>0.02</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>0.5</v>
       </c>
       <c r="E10" s="3">
@@ -1175,13 +1196,13 @@
       <c r="A11">
         <v>-40</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>0.29999999999999999</v>
       </c>
       <c r="C11" s="4">
         <v>0.01</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>0.19</v>
       </c>
       <c r="E11" s="3">
@@ -1192,13 +1213,13 @@
       <c r="A12">
         <v>-50</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>0.11</v>
       </c>
       <c r="C12" s="4">
         <v>0.01</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>0.029999999999999999</v>
       </c>
       <c r="E12" s="3">
@@ -1220,7 +1241,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1230,75 +1251,89 @@
     <col customWidth="1" min="4" max="4" width="30.8515625"/>
     <col customWidth="1" min="5" max="6" width="11.7109375"/>
     <col customWidth="1" min="7" max="7" width="17.28125"/>
+    <col customWidth="1" min="9" max="9" width="14.7109375"/>
+    <col customWidth="1" min="10" max="10" width="12.7109375"/>
+    <col customWidth="1" min="11" max="11" width="13.00390625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H1"/>
+      <c r="I1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="10">
         <v>54</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>3.3399999999999999</v>
       </c>
-      <c r="C2" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="D2" s="11">
+      <c r="C2" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="D2" s="10">
         <v>53.299999999999997</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="6">
         <v>3.5299999999999998</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="6">
         <v>0.02</v>
       </c>
       <c r="G2">
         <v>100</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="10">
         <v>52.600000000000001</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>3.27</v>
       </c>
-      <c r="C3" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="D3" s="11">
+      <c r="C3" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="D3" s="10">
         <v>51.899999999999999</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="6">
         <v>3.3799999999999999</v>
       </c>
-      <c r="F3" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="F3" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="G3" s="1">
         <v>100</v>
       </c>
     </row>
@@ -1306,22 +1341,22 @@
       <c r="A4" s="10">
         <v>51.200000000000003</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>3.2000000000000002</v>
       </c>
-      <c r="C4" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="D4" s="11">
+      <c r="C4" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="D4" s="10">
         <v>50.5</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="6">
         <v>3.2799999999999998</v>
       </c>
-      <c r="F4" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="G4" s="5">
+      <c r="F4" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="G4" s="1">
         <v>100</v>
       </c>
     </row>
@@ -1329,22 +1364,22 @@
       <c r="A5" s="10">
         <v>49.799999999999997</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>3.1299999999999999</v>
       </c>
-      <c r="C5" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="D5" s="11">
+      <c r="C5" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="D5" s="10">
         <v>49.100000000000001</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="6">
         <v>3.2000000000000002</v>
       </c>
-      <c r="F5" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="G5" s="5">
+      <c r="F5" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="G5" s="1">
         <v>100</v>
       </c>
     </row>
@@ -1352,22 +1387,22 @@
       <c r="A6" s="10">
         <v>48.399999999999999</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>3.0499999999999998</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>0.02</v>
       </c>
       <c r="D6" s="10">
         <v>47.700000000000003</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>3.1000000000000001</v>
       </c>
-      <c r="F6" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="G6" s="5">
+      <c r="F6" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="G6" s="1">
         <v>100</v>
       </c>
     </row>
@@ -1375,22 +1410,22 @@
       <c r="A7" s="10">
         <v>47</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>2.9399999999999999</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>0.02</v>
       </c>
       <c r="D7" s="10">
         <v>46.299999999999997</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>3</v>
       </c>
-      <c r="F7" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="G7" s="5">
+      <c r="F7" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="G7" s="1">
         <v>100</v>
       </c>
     </row>
@@ -1398,22 +1433,22 @@
       <c r="A8" s="10">
         <v>45.600000000000001</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>2.8500000000000001</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>0.02</v>
       </c>
       <c r="D8" s="10">
         <v>45</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>1.9199999999999999</v>
       </c>
-      <c r="F8" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="G8" s="5">
+      <c r="F8" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="G8" s="1">
         <v>100</v>
       </c>
     </row>
@@ -1421,42 +1456,42 @@
       <c r="A9" s="10">
         <v>44.200000000000003</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>2.7400000000000002</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>0.02</v>
       </c>
       <c r="D9" s="10">
         <v>43.5</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>2.8199999999999998</v>
       </c>
-      <c r="F9" s="7">
-        <v>0.02</v>
-      </c>
-      <c r="G9" s="5">
+      <c r="F9" s="6">
+        <v>0.02</v>
+      </c>
+      <c r="G9" s="1">
         <v>100</v>
       </c>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="13">
+      <c r="A10" s="11">
         <v>46.799999999999997</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="12">
         <v>4.1299999999999999</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="12">
         <v>0.02</v>
       </c>
       <c r="D10" s="10">
         <v>47.5</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>4.9000000000000004</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>0.02</v>
       </c>
       <c r="G10">
@@ -1464,22 +1499,22 @@
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="13">
+      <c r="A11" s="11">
         <v>45.399999999999999</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="12">
         <v>4.0300000000000002</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="12">
         <v>0.01</v>
       </c>
       <c r="D11" s="10">
         <v>46.100000000000001</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>4.6799999999999997</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>0.02</v>
       </c>
       <c r="G11">
@@ -1487,22 +1522,22 @@
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="13">
+      <c r="A12" s="11">
         <v>44</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="12">
         <v>3.96</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="12">
         <v>0.02</v>
       </c>
       <c r="D12" s="10">
         <v>44.600000000000001</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>4.54</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>0.01</v>
       </c>
       <c r="G12">
@@ -1510,22 +1545,22 @@
       </c>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13" s="13">
+      <c r="A13" s="11">
         <v>42.5</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="12">
         <v>3.8100000000000001</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="12">
         <v>0.01</v>
       </c>
       <c r="D13" s="10">
         <v>43.299999999999997</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>4.3799999999999999</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>0.02</v>
       </c>
       <c r="G13">
@@ -1533,22 +1568,22 @@
       </c>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="13">
+      <c r="A14" s="11">
         <v>41</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="12">
         <v>3.7599999999999998</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="12">
         <v>0.02</v>
       </c>
       <c r="D14" s="10">
         <v>41.899999999999999</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>4.3600000000000003</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>0.01</v>
       </c>
       <c r="G14">
@@ -1556,22 +1591,22 @@
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="A15" s="13">
+      <c r="A15" s="11">
         <v>39.600000000000001</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="12">
         <v>3.6800000000000002</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="12">
         <v>0.02</v>
       </c>
       <c r="D15" s="10">
         <v>40.399999999999999</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>4.25</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>0.02</v>
       </c>
       <c r="G15">
@@ -1579,22 +1614,22 @@
       </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="13">
+      <c r="A16" s="11">
         <v>38.200000000000003</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="12">
         <v>3.5499999999999998</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="12">
         <v>0.02</v>
       </c>
       <c r="D16" s="10">
         <v>38.899999999999999</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>4.04</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>0.02</v>
       </c>
       <c r="G16">
@@ -1602,22 +1637,22 @@
       </c>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="13">
+      <c r="A17" s="11">
         <v>36.799999999999997</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="12">
         <v>3.4700000000000002</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="12">
         <v>0.02</v>
       </c>
       <c r="D17" s="10">
         <v>37.5</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>3.8500000000000001</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>0.02</v>
       </c>
       <c r="G17">
@@ -1625,22 +1660,22 @@
       </c>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="13">
+      <c r="A18" s="11">
         <v>35.399999999999999</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="12">
         <v>3.3900000000000001</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="12">
         <v>0.02</v>
       </c>
       <c r="D18" s="10">
         <v>36</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>3.7000000000000002</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>0.02</v>
       </c>
       <c r="G18">
@@ -1651,10 +1686,10 @@
       <c r="D19" s="10">
         <v>34.600000000000001</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>3.6200000000000001</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>0.02</v>
       </c>
       <c r="G19">

</xml_diff>